<commit_message>
Main.c file upload Prac4
</commit_message>
<xml_diff>
--- a/3096-Pracs-NRTKAM001/Prac 4/LUT values and plots.xlsx
+++ b/3096-Pracs-NRTKAM001/Prac 4/LUT values and plots.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/acef92bacdd726a6/Documents/2022/Semester 2/EEE3096S - Embedded Systems II/GIT/EEE3096S_EmbeddedSystemsII/3096-Pracs-NRTKAM001/Prac 4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{27C005D4-0D88-489C-9CFB-E51BF442A67B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="8_{27C005D4-0D88-489C-9CFB-E51BF442A67B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2BFD98F8-29A0-4634-9F01-D625BF42A557}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10530" xr2:uid="{05097434-5E90-4613-B800-A84DB81873BC}"/>
   </bookViews>
@@ -61,7 +61,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="170" formatCode="0\,"/>
+    <numFmt numFmtId="164" formatCode="0\,"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -92,12 +92,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2183,7 +2182,7 @@
                 </c:marker>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$B$2:$B$129</c15:sqref>
@@ -2581,7 +2580,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000000-5C76-49BB-AD79-F46DF19CE797}"/>
                   </c:ext>
@@ -4128,7 +4127,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000002-37B5-4618-884C-11E72B10ED0B}"/>
                   </c:ext>
@@ -4156,7 +4155,7 @@
                 </c:marker>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$C$2:$C$129</c15:sqref>
@@ -4554,7 +4553,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000000-37B5-4618-884C-11E72B10ED0B}"/>
                   </c:ext>
@@ -6837,21 +6836,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E418BC2B-D97C-4632-B73C-2AC834C3CF6D}">
-  <dimension ref="A1:H129"/>
+  <dimension ref="A1:J129"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H1048576"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
     <col min="2" max="2" width="8.7265625" style="1"/>
-    <col min="6" max="6" width="10.08984375" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.2265625" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.7265625" style="4"/>
+    <col min="6" max="6" width="10.08984375" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.2265625" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.7265625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6864,358 +6863,366 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="J1" t="str">
+        <f>_xlfn.TEXTJOIN(",",,G2:G129)</f>
+        <v>16,32,48,64,80,96,112,128,144,160,176,192,208,224,240,256,272,288,304,320,336,352,368,384,400,416,432,448,464,480,496,512,527,543,559,575,591,607,623,639,655,671,687,703,719,735,751,767,783,799,815,831,847,863,879,895,911,927,943,959,975,991,1007,1023,1007,991,975,959,943,927,911,895,879,863,847,831,815,799,783,767,751,735,719,703,687,671,655,639,623,607,591,575,559,543,527,512,496,480,464,448,432,416,400,384,368,352,336,320,304,288,272,256,240,224,208,192,176,160,144,128,112,96,80,64,48,32,16,0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="2">
         <v>512</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2">
         <v>16</v>
       </c>
       <c r="D2">
         <v>0</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2" s="3">
         <v>512</v>
       </c>
-      <c r="G2" s="4">
+      <c r="G2" s="3">
         <v>16</v>
       </c>
-      <c r="H2" s="4">
+      <c r="H2" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="J2" t="str">
+        <f>_xlfn.TEXTJOIN(",",,H2:H129)</f>
+        <v>0,8,16,24,32,40,48,56,64,72,80,88,96,104,112,120,128,136,144,152,160,168,176,184,192,200,208,216,224,232,240,248,256,264,272,280,288,296,304,312,320,328,336,344,352,360,368,376,384,392,400,408,416,424,432,440,448,456,464,472,480,488,496,504,512,520,528,536,544,552,560,568,576,584,592,600,608,616,624,632,640,648,656,664,672,680,688,696,704,712,720,728,736,744,752,760,768,776,784,792,800,808,816,824,832,840,848,856,864,872,880,888,896,904,912,920,928,936,944,952,960,968,976,984,992,1000,1008,1016</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3">
         <v>537</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3">
         <v>32</v>
       </c>
       <c r="D3">
         <v>8</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="3">
         <v>537</v>
       </c>
-      <c r="G3" s="4">
+      <c r="G3" s="3">
         <v>32</v>
       </c>
-      <c r="H3" s="4">
+      <c r="H3" s="3">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4">
         <v>562</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4">
         <v>48</v>
       </c>
       <c r="D4">
         <v>16</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="3">
         <v>562</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4" s="3">
         <v>48</v>
       </c>
-      <c r="H4" s="4">
+      <c r="H4" s="3">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5">
         <v>587</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5">
         <v>64</v>
       </c>
       <c r="D5">
         <v>24</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="3">
         <v>587</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5" s="3">
         <v>64</v>
       </c>
-      <c r="H5" s="4">
+      <c r="H5" s="3">
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6">
         <v>611</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6">
         <v>80</v>
       </c>
       <c r="D6">
         <v>32</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="3">
         <v>611</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6" s="3">
         <v>80</v>
       </c>
-      <c r="H6" s="4">
+      <c r="H6" s="3">
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A7" s="1">
         <v>6</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7">
         <v>636</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7">
         <v>96</v>
       </c>
       <c r="D7">
         <v>40</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7" s="3">
         <v>636</v>
       </c>
-      <c r="G7" s="4">
+      <c r="G7" s="3">
         <v>96</v>
       </c>
-      <c r="H7" s="4">
+      <c r="H7" s="3">
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A8" s="1">
         <v>7</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8">
         <v>660</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8">
         <v>112</v>
       </c>
       <c r="D8">
         <v>48</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F8" s="3">
         <v>660</v>
       </c>
-      <c r="G8" s="4">
+      <c r="G8" s="3">
         <v>112</v>
       </c>
-      <c r="H8" s="4">
+      <c r="H8" s="3">
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A9" s="1">
         <v>8</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9">
         <v>684</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9">
         <v>128</v>
       </c>
       <c r="D9">
         <v>56</v>
       </c>
-      <c r="F9" s="4">
+      <c r="F9" s="3">
         <v>684</v>
       </c>
-      <c r="G9" s="4">
+      <c r="G9" s="3">
         <v>128</v>
       </c>
-      <c r="H9" s="4">
+      <c r="H9" s="3">
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A10" s="1">
         <v>9</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10">
         <v>707</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10">
         <v>144</v>
       </c>
       <c r="D10">
         <v>64</v>
       </c>
-      <c r="F10" s="4">
+      <c r="F10" s="3">
         <v>707</v>
       </c>
-      <c r="G10" s="4">
+      <c r="G10" s="3">
         <v>144</v>
       </c>
-      <c r="H10" s="4">
+      <c r="H10" s="3">
         <v>64</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A11" s="1">
         <v>10</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11">
         <v>730</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11">
         <v>160</v>
       </c>
       <c r="D11">
         <v>72</v>
       </c>
-      <c r="F11" s="4">
+      <c r="F11" s="3">
         <v>730</v>
       </c>
-      <c r="G11" s="4">
+      <c r="G11" s="3">
         <v>160</v>
       </c>
-      <c r="H11" s="4">
+      <c r="H11" s="3">
         <v>72</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A12" s="1">
         <v>11</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12">
         <v>753</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12">
         <v>176</v>
       </c>
       <c r="D12">
         <v>80</v>
       </c>
-      <c r="F12" s="4">
+      <c r="F12" s="3">
         <v>753</v>
       </c>
-      <c r="G12" s="4">
+      <c r="G12" s="3">
         <v>176</v>
       </c>
-      <c r="H12" s="4">
+      <c r="H12" s="3">
         <v>80</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A13" s="1">
         <v>12</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13">
         <v>774</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13">
         <v>192</v>
       </c>
       <c r="D13">
         <v>88</v>
       </c>
-      <c r="F13" s="4">
+      <c r="F13" s="3">
         <v>774</v>
       </c>
-      <c r="G13" s="4">
+      <c r="G13" s="3">
         <v>192</v>
       </c>
-      <c r="H13" s="4">
+      <c r="H13" s="3">
         <v>88</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A14" s="1">
         <v>13</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14">
         <v>796</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14">
         <v>208</v>
       </c>
       <c r="D14">
         <v>96</v>
       </c>
-      <c r="F14" s="4">
+      <c r="F14" s="3">
         <v>796</v>
       </c>
-      <c r="G14" s="4">
+      <c r="G14" s="3">
         <v>208</v>
       </c>
-      <c r="H14" s="4">
+      <c r="H14" s="3">
         <v>96</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A15" s="1">
         <v>14</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15">
         <v>816</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15">
         <v>224</v>
       </c>
       <c r="D15">
         <v>104</v>
       </c>
-      <c r="F15" s="4">
+      <c r="F15" s="3">
         <v>816</v>
       </c>
-      <c r="G15" s="4">
+      <c r="G15" s="3">
         <v>224</v>
       </c>
-      <c r="H15" s="4">
+      <c r="H15" s="3">
         <v>104</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A16" s="1">
         <v>15</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B16">
         <v>836</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16">
         <v>240</v>
       </c>
       <c r="D16">
         <v>112</v>
       </c>
-      <c r="F16" s="4">
+      <c r="F16" s="3">
         <v>836</v>
       </c>
-      <c r="G16" s="4">
+      <c r="G16" s="3">
         <v>240</v>
       </c>
-      <c r="H16" s="4">
+      <c r="H16" s="3">
         <v>112</v>
       </c>
     </row>
@@ -7223,22 +7230,22 @@
       <c r="A17" s="1">
         <v>16</v>
       </c>
-      <c r="B17" s="2">
+      <c r="B17">
         <v>855</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17">
         <v>256</v>
       </c>
       <c r="D17">
         <v>120</v>
       </c>
-      <c r="F17" s="4">
+      <c r="F17" s="3">
         <v>855</v>
       </c>
-      <c r="G17" s="4">
+      <c r="G17" s="3">
         <v>256</v>
       </c>
-      <c r="H17" s="4">
+      <c r="H17" s="3">
         <v>120</v>
       </c>
     </row>
@@ -7246,22 +7253,22 @@
       <c r="A18" s="1">
         <v>17</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B18">
         <v>873</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C18">
         <v>272</v>
       </c>
       <c r="D18">
         <v>128</v>
       </c>
-      <c r="F18" s="4">
+      <c r="F18" s="3">
         <v>873</v>
       </c>
-      <c r="G18" s="4">
+      <c r="G18" s="3">
         <v>272</v>
       </c>
-      <c r="H18" s="4">
+      <c r="H18" s="3">
         <v>128</v>
       </c>
     </row>
@@ -7269,22 +7276,22 @@
       <c r="A19" s="1">
         <v>18</v>
       </c>
-      <c r="B19" s="2">
+      <c r="B19">
         <v>890</v>
       </c>
-      <c r="C19" s="2">
+      <c r="C19">
         <v>288</v>
       </c>
       <c r="D19">
         <v>136</v>
       </c>
-      <c r="F19" s="4">
+      <c r="F19" s="3">
         <v>890</v>
       </c>
-      <c r="G19" s="4">
+      <c r="G19" s="3">
         <v>288</v>
       </c>
-      <c r="H19" s="4">
+      <c r="H19" s="3">
         <v>136</v>
       </c>
     </row>
@@ -7292,22 +7299,22 @@
       <c r="A20" s="1">
         <v>19</v>
       </c>
-      <c r="B20" s="2">
+      <c r="B20">
         <v>907</v>
       </c>
-      <c r="C20" s="2">
+      <c r="C20">
         <v>304</v>
       </c>
       <c r="D20">
         <v>144</v>
       </c>
-      <c r="F20" s="4">
+      <c r="F20" s="3">
         <v>907</v>
       </c>
-      <c r="G20" s="4">
+      <c r="G20" s="3">
         <v>304</v>
       </c>
-      <c r="H20" s="4">
+      <c r="H20" s="3">
         <v>144</v>
       </c>
     </row>
@@ -7315,22 +7322,22 @@
       <c r="A21" s="1">
         <v>20</v>
       </c>
-      <c r="B21" s="2">
+      <c r="B21">
         <v>922</v>
       </c>
-      <c r="C21" s="2">
+      <c r="C21">
         <v>320</v>
       </c>
       <c r="D21">
         <v>152</v>
       </c>
-      <c r="F21" s="4">
+      <c r="F21" s="3">
         <v>922</v>
       </c>
-      <c r="G21" s="4">
+      <c r="G21" s="3">
         <v>320</v>
       </c>
-      <c r="H21" s="4">
+      <c r="H21" s="3">
         <v>152</v>
       </c>
     </row>
@@ -7338,22 +7345,22 @@
       <c r="A22" s="1">
         <v>21</v>
       </c>
-      <c r="B22" s="2">
+      <c r="B22">
         <v>937</v>
       </c>
-      <c r="C22" s="2">
+      <c r="C22">
         <v>336</v>
       </c>
       <c r="D22">
         <v>160</v>
       </c>
-      <c r="F22" s="4">
+      <c r="F22" s="3">
         <v>937</v>
       </c>
-      <c r="G22" s="4">
+      <c r="G22" s="3">
         <v>336</v>
       </c>
-      <c r="H22" s="4">
+      <c r="H22" s="3">
         <v>160</v>
       </c>
     </row>
@@ -7361,22 +7368,22 @@
       <c r="A23" s="1">
         <v>22</v>
       </c>
-      <c r="B23" s="2">
+      <c r="B23">
         <v>950</v>
       </c>
-      <c r="C23" s="2">
+      <c r="C23">
         <v>352</v>
       </c>
       <c r="D23">
         <v>168</v>
       </c>
-      <c r="F23" s="4">
+      <c r="F23" s="3">
         <v>950</v>
       </c>
-      <c r="G23" s="4">
+      <c r="G23" s="3">
         <v>352</v>
       </c>
-      <c r="H23" s="4">
+      <c r="H23" s="3">
         <v>168</v>
       </c>
     </row>
@@ -7384,22 +7391,22 @@
       <c r="A24" s="1">
         <v>23</v>
       </c>
-      <c r="B24" s="2">
+      <c r="B24">
         <v>963</v>
       </c>
-      <c r="C24" s="2">
+      <c r="C24">
         <v>368</v>
       </c>
       <c r="D24">
         <v>176</v>
       </c>
-      <c r="F24" s="4">
+      <c r="F24" s="3">
         <v>963</v>
       </c>
-      <c r="G24" s="4">
+      <c r="G24" s="3">
         <v>368</v>
       </c>
-      <c r="H24" s="4">
+      <c r="H24" s="3">
         <v>176</v>
       </c>
     </row>
@@ -7407,22 +7414,22 @@
       <c r="A25" s="1">
         <v>24</v>
       </c>
-      <c r="B25" s="2">
+      <c r="B25">
         <v>974</v>
       </c>
-      <c r="C25" s="2">
+      <c r="C25">
         <v>384</v>
       </c>
       <c r="D25">
         <v>184</v>
       </c>
-      <c r="F25" s="4">
+      <c r="F25" s="3">
         <v>974</v>
       </c>
-      <c r="G25" s="4">
+      <c r="G25" s="3">
         <v>384</v>
       </c>
-      <c r="H25" s="4">
+      <c r="H25" s="3">
         <v>184</v>
       </c>
     </row>
@@ -7430,22 +7437,22 @@
       <c r="A26" s="1">
         <v>25</v>
       </c>
-      <c r="B26" s="2">
+      <c r="B26">
         <v>984</v>
       </c>
-      <c r="C26" s="2">
+      <c r="C26">
         <v>400</v>
       </c>
       <c r="D26">
         <v>192</v>
       </c>
-      <c r="F26" s="4">
+      <c r="F26" s="3">
         <v>984</v>
       </c>
-      <c r="G26" s="4">
+      <c r="G26" s="3">
         <v>400</v>
       </c>
-      <c r="H26" s="4">
+      <c r="H26" s="3">
         <v>192</v>
       </c>
     </row>
@@ -7453,22 +7460,22 @@
       <c r="A27" s="1">
         <v>26</v>
       </c>
-      <c r="B27" s="2">
+      <c r="B27">
         <v>993</v>
       </c>
-      <c r="C27" s="2">
+      <c r="C27">
         <v>416</v>
       </c>
       <c r="D27">
         <v>200</v>
       </c>
-      <c r="F27" s="4">
+      <c r="F27" s="3">
         <v>993</v>
       </c>
-      <c r="G27" s="4">
+      <c r="G27" s="3">
         <v>416</v>
       </c>
-      <c r="H27" s="4">
+      <c r="H27" s="3">
         <v>200</v>
       </c>
     </row>
@@ -7476,22 +7483,22 @@
       <c r="A28" s="1">
         <v>27</v>
       </c>
-      <c r="B28" s="2">
+      <c r="B28">
         <v>1001</v>
       </c>
-      <c r="C28" s="2">
+      <c r="C28">
         <v>432</v>
       </c>
       <c r="D28">
         <v>208</v>
       </c>
-      <c r="F28" s="4">
+      <c r="F28" s="3">
         <v>1001</v>
       </c>
-      <c r="G28" s="4">
+      <c r="G28" s="3">
         <v>432</v>
       </c>
-      <c r="H28" s="4">
+      <c r="H28" s="3">
         <v>208</v>
       </c>
     </row>
@@ -7499,22 +7506,22 @@
       <c r="A29" s="1">
         <v>28</v>
       </c>
-      <c r="B29" s="2">
+      <c r="B29">
         <v>1008</v>
       </c>
-      <c r="C29" s="2">
+      <c r="C29">
         <v>448</v>
       </c>
       <c r="D29">
         <v>216</v>
       </c>
-      <c r="F29" s="4">
+      <c r="F29" s="3">
         <v>1008</v>
       </c>
-      <c r="G29" s="4">
+      <c r="G29" s="3">
         <v>448</v>
       </c>
-      <c r="H29" s="4">
+      <c r="H29" s="3">
         <v>216</v>
       </c>
     </row>
@@ -7522,22 +7529,22 @@
       <c r="A30" s="1">
         <v>29</v>
       </c>
-      <c r="B30" s="2">
+      <c r="B30">
         <v>1013</v>
       </c>
-      <c r="C30" s="2">
+      <c r="C30">
         <v>464</v>
       </c>
       <c r="D30">
         <v>224</v>
       </c>
-      <c r="F30" s="4">
+      <c r="F30" s="3">
         <v>1013</v>
       </c>
-      <c r="G30" s="4">
+      <c r="G30" s="3">
         <v>464</v>
       </c>
-      <c r="H30" s="4">
+      <c r="H30" s="3">
         <v>224</v>
       </c>
     </row>
@@ -7545,22 +7552,22 @@
       <c r="A31" s="1">
         <v>30</v>
       </c>
-      <c r="B31" s="2">
+      <c r="B31">
         <v>1017</v>
       </c>
-      <c r="C31" s="2">
+      <c r="C31">
         <v>480</v>
       </c>
       <c r="D31">
         <v>232</v>
       </c>
-      <c r="F31" s="4">
+      <c r="F31" s="3">
         <v>1017</v>
       </c>
-      <c r="G31" s="4">
+      <c r="G31" s="3">
         <v>480</v>
       </c>
-      <c r="H31" s="4">
+      <c r="H31" s="3">
         <v>232</v>
       </c>
     </row>
@@ -7568,22 +7575,22 @@
       <c r="A32" s="1">
         <v>31</v>
       </c>
-      <c r="B32" s="2">
+      <c r="B32">
         <v>1021</v>
       </c>
-      <c r="C32" s="2">
+      <c r="C32">
         <v>496</v>
       </c>
       <c r="D32">
         <v>240</v>
       </c>
-      <c r="F32" s="4">
+      <c r="F32" s="3">
         <v>1021</v>
       </c>
-      <c r="G32" s="4">
+      <c r="G32" s="3">
         <v>496</v>
       </c>
-      <c r="H32" s="4">
+      <c r="H32" s="3">
         <v>240</v>
       </c>
     </row>
@@ -7591,22 +7598,22 @@
       <c r="A33" s="1">
         <v>32</v>
       </c>
-      <c r="B33" s="2">
+      <c r="B33">
         <v>1022</v>
       </c>
-      <c r="C33" s="2">
+      <c r="C33">
         <v>512</v>
       </c>
       <c r="D33">
         <v>248</v>
       </c>
-      <c r="F33" s="4">
+      <c r="F33" s="3">
         <v>1022</v>
       </c>
-      <c r="G33" s="4">
+      <c r="G33" s="3">
         <v>512</v>
       </c>
-      <c r="H33" s="4">
+      <c r="H33" s="3">
         <v>248</v>
       </c>
     </row>
@@ -7614,22 +7621,22 @@
       <c r="A34" s="1">
         <v>33</v>
       </c>
-      <c r="B34" s="2">
+      <c r="B34">
         <v>1023</v>
       </c>
-      <c r="C34" s="2">
+      <c r="C34">
         <v>527</v>
       </c>
       <c r="D34">
         <v>256</v>
       </c>
-      <c r="F34" s="4">
+      <c r="F34" s="3">
         <v>1023</v>
       </c>
-      <c r="G34" s="4">
+      <c r="G34" s="3">
         <v>527</v>
       </c>
-      <c r="H34" s="4">
+      <c r="H34" s="3">
         <v>256</v>
       </c>
     </row>
@@ -7637,22 +7644,22 @@
       <c r="A35" s="1">
         <v>34</v>
       </c>
-      <c r="B35" s="2">
+      <c r="B35">
         <v>1022</v>
       </c>
-      <c r="C35" s="2">
+      <c r="C35">
         <v>543</v>
       </c>
       <c r="D35">
         <v>264</v>
       </c>
-      <c r="F35" s="4">
+      <c r="F35" s="3">
         <v>1022</v>
       </c>
-      <c r="G35" s="4">
+      <c r="G35" s="3">
         <v>543</v>
       </c>
-      <c r="H35" s="4">
+      <c r="H35" s="3">
         <v>264</v>
       </c>
     </row>
@@ -7660,22 +7667,22 @@
       <c r="A36" s="1">
         <v>35</v>
       </c>
-      <c r="B36" s="2">
+      <c r="B36">
         <v>1021</v>
       </c>
-      <c r="C36" s="2">
+      <c r="C36">
         <v>559</v>
       </c>
       <c r="D36">
         <v>272</v>
       </c>
-      <c r="F36" s="4">
+      <c r="F36" s="3">
         <v>1021</v>
       </c>
-      <c r="G36" s="4">
+      <c r="G36" s="3">
         <v>559</v>
       </c>
-      <c r="H36" s="4">
+      <c r="H36" s="3">
         <v>272</v>
       </c>
     </row>
@@ -7683,22 +7690,22 @@
       <c r="A37" s="1">
         <v>36</v>
       </c>
-      <c r="B37" s="2">
+      <c r="B37">
         <v>1017</v>
       </c>
-      <c r="C37" s="2">
+      <c r="C37">
         <v>575</v>
       </c>
       <c r="D37">
         <v>280</v>
       </c>
-      <c r="F37" s="4">
+      <c r="F37" s="3">
         <v>1017</v>
       </c>
-      <c r="G37" s="4">
+      <c r="G37" s="3">
         <v>575</v>
       </c>
-      <c r="H37" s="4">
+      <c r="H37" s="3">
         <v>280</v>
       </c>
     </row>
@@ -7706,22 +7713,22 @@
       <c r="A38" s="1">
         <v>37</v>
       </c>
-      <c r="B38" s="2">
+      <c r="B38">
         <v>1013</v>
       </c>
-      <c r="C38" s="2">
+      <c r="C38">
         <v>591</v>
       </c>
       <c r="D38">
         <v>288</v>
       </c>
-      <c r="F38" s="4">
+      <c r="F38" s="3">
         <v>1013</v>
       </c>
-      <c r="G38" s="4">
+      <c r="G38" s="3">
         <v>591</v>
       </c>
-      <c r="H38" s="4">
+      <c r="H38" s="3">
         <v>288</v>
       </c>
     </row>
@@ -7729,22 +7736,22 @@
       <c r="A39" s="1">
         <v>38</v>
       </c>
-      <c r="B39" s="2">
+      <c r="B39">
         <v>1008</v>
       </c>
-      <c r="C39" s="2">
+      <c r="C39">
         <v>607</v>
       </c>
       <c r="D39">
         <v>296</v>
       </c>
-      <c r="F39" s="4">
+      <c r="F39" s="3">
         <v>1008</v>
       </c>
-      <c r="G39" s="4">
+      <c r="G39" s="3">
         <v>607</v>
       </c>
-      <c r="H39" s="4">
+      <c r="H39" s="3">
         <v>296</v>
       </c>
     </row>
@@ -7752,22 +7759,22 @@
       <c r="A40" s="1">
         <v>39</v>
       </c>
-      <c r="B40" s="2">
+      <c r="B40">
         <v>1001</v>
       </c>
-      <c r="C40" s="2">
+      <c r="C40">
         <v>623</v>
       </c>
       <c r="D40">
         <v>304</v>
       </c>
-      <c r="F40" s="4">
+      <c r="F40" s="3">
         <v>1001</v>
       </c>
-      <c r="G40" s="4">
+      <c r="G40" s="3">
         <v>623</v>
       </c>
-      <c r="H40" s="4">
+      <c r="H40" s="3">
         <v>304</v>
       </c>
     </row>
@@ -7775,22 +7782,22 @@
       <c r="A41" s="1">
         <v>40</v>
       </c>
-      <c r="B41" s="2">
+      <c r="B41">
         <v>993</v>
       </c>
-      <c r="C41" s="2">
+      <c r="C41">
         <v>639</v>
       </c>
       <c r="D41">
         <v>312</v>
       </c>
-      <c r="F41" s="4">
+      <c r="F41" s="3">
         <v>993</v>
       </c>
-      <c r="G41" s="4">
+      <c r="G41" s="3">
         <v>639</v>
       </c>
-      <c r="H41" s="4">
+      <c r="H41" s="3">
         <v>312</v>
       </c>
     </row>
@@ -7798,22 +7805,22 @@
       <c r="A42" s="1">
         <v>41</v>
       </c>
-      <c r="B42" s="2">
+      <c r="B42">
         <v>984</v>
       </c>
-      <c r="C42" s="2">
+      <c r="C42">
         <v>655</v>
       </c>
       <c r="D42">
         <v>320</v>
       </c>
-      <c r="F42" s="4">
+      <c r="F42" s="3">
         <v>984</v>
       </c>
-      <c r="G42" s="4">
+      <c r="G42" s="3">
         <v>655</v>
       </c>
-      <c r="H42" s="4">
+      <c r="H42" s="3">
         <v>320</v>
       </c>
     </row>
@@ -7821,22 +7828,22 @@
       <c r="A43" s="1">
         <v>42</v>
       </c>
-      <c r="B43" s="2">
+      <c r="B43">
         <v>974</v>
       </c>
-      <c r="C43" s="2">
+      <c r="C43">
         <v>671</v>
       </c>
       <c r="D43">
         <v>328</v>
       </c>
-      <c r="F43" s="4">
+      <c r="F43" s="3">
         <v>974</v>
       </c>
-      <c r="G43" s="4">
+      <c r="G43" s="3">
         <v>671</v>
       </c>
-      <c r="H43" s="4">
+      <c r="H43" s="3">
         <v>328</v>
       </c>
     </row>
@@ -7844,22 +7851,22 @@
       <c r="A44" s="1">
         <v>43</v>
       </c>
-      <c r="B44" s="2">
+      <c r="B44">
         <v>963</v>
       </c>
-      <c r="C44" s="2">
+      <c r="C44">
         <v>687</v>
       </c>
       <c r="D44">
         <v>336</v>
       </c>
-      <c r="F44" s="4">
+      <c r="F44" s="3">
         <v>963</v>
       </c>
-      <c r="G44" s="4">
+      <c r="G44" s="3">
         <v>687</v>
       </c>
-      <c r="H44" s="4">
+      <c r="H44" s="3">
         <v>336</v>
       </c>
     </row>
@@ -7867,22 +7874,22 @@
       <c r="A45" s="1">
         <v>44</v>
       </c>
-      <c r="B45" s="2">
+      <c r="B45">
         <v>950</v>
       </c>
-      <c r="C45" s="2">
+      <c r="C45">
         <v>703</v>
       </c>
       <c r="D45">
         <v>344</v>
       </c>
-      <c r="F45" s="4">
+      <c r="F45" s="3">
         <v>950</v>
       </c>
-      <c r="G45" s="4">
+      <c r="G45" s="3">
         <v>703</v>
       </c>
-      <c r="H45" s="4">
+      <c r="H45" s="3">
         <v>344</v>
       </c>
     </row>
@@ -7890,22 +7897,22 @@
       <c r="A46" s="1">
         <v>45</v>
       </c>
-      <c r="B46" s="2">
+      <c r="B46">
         <v>937</v>
       </c>
-      <c r="C46" s="2">
+      <c r="C46">
         <v>719</v>
       </c>
       <c r="D46">
         <v>352</v>
       </c>
-      <c r="F46" s="4">
+      <c r="F46" s="3">
         <v>937</v>
       </c>
-      <c r="G46" s="4">
+      <c r="G46" s="3">
         <v>719</v>
       </c>
-      <c r="H46" s="4">
+      <c r="H46" s="3">
         <v>352</v>
       </c>
     </row>
@@ -7913,22 +7920,22 @@
       <c r="A47" s="1">
         <v>46</v>
       </c>
-      <c r="B47" s="2">
+      <c r="B47">
         <v>922</v>
       </c>
-      <c r="C47" s="2">
+      <c r="C47">
         <v>735</v>
       </c>
       <c r="D47">
         <v>360</v>
       </c>
-      <c r="F47" s="4">
+      <c r="F47" s="3">
         <v>922</v>
       </c>
-      <c r="G47" s="4">
+      <c r="G47" s="3">
         <v>735</v>
       </c>
-      <c r="H47" s="4">
+      <c r="H47" s="3">
         <v>360</v>
       </c>
     </row>
@@ -7936,22 +7943,22 @@
       <c r="A48" s="1">
         <v>47</v>
       </c>
-      <c r="B48" s="2">
+      <c r="B48">
         <v>907</v>
       </c>
-      <c r="C48" s="2">
+      <c r="C48">
         <v>751</v>
       </c>
       <c r="D48">
         <v>368</v>
       </c>
-      <c r="F48" s="4">
+      <c r="F48" s="3">
         <v>907</v>
       </c>
-      <c r="G48" s="4">
+      <c r="G48" s="3">
         <v>751</v>
       </c>
-      <c r="H48" s="4">
+      <c r="H48" s="3">
         <v>368</v>
       </c>
     </row>
@@ -7959,22 +7966,22 @@
       <c r="A49" s="1">
         <v>48</v>
       </c>
-      <c r="B49" s="2">
+      <c r="B49">
         <v>890</v>
       </c>
-      <c r="C49" s="2">
+      <c r="C49">
         <v>767</v>
       </c>
       <c r="D49">
         <v>376</v>
       </c>
-      <c r="F49" s="4">
+      <c r="F49" s="3">
         <v>890</v>
       </c>
-      <c r="G49" s="4">
+      <c r="G49" s="3">
         <v>767</v>
       </c>
-      <c r="H49" s="4">
+      <c r="H49" s="3">
         <v>376</v>
       </c>
     </row>
@@ -7982,22 +7989,22 @@
       <c r="A50" s="1">
         <v>49</v>
       </c>
-      <c r="B50" s="2">
+      <c r="B50">
         <v>873</v>
       </c>
-      <c r="C50" s="2">
+      <c r="C50">
         <v>783</v>
       </c>
       <c r="D50">
         <v>384</v>
       </c>
-      <c r="F50" s="4">
+      <c r="F50" s="3">
         <v>873</v>
       </c>
-      <c r="G50" s="4">
+      <c r="G50" s="3">
         <v>783</v>
       </c>
-      <c r="H50" s="4">
+      <c r="H50" s="3">
         <v>384</v>
       </c>
     </row>
@@ -8005,22 +8012,22 @@
       <c r="A51" s="1">
         <v>50</v>
       </c>
-      <c r="B51" s="2">
+      <c r="B51">
         <v>855</v>
       </c>
-      <c r="C51" s="2">
+      <c r="C51">
         <v>799</v>
       </c>
       <c r="D51">
         <v>392</v>
       </c>
-      <c r="F51" s="4">
+      <c r="F51" s="3">
         <v>855</v>
       </c>
-      <c r="G51" s="4">
+      <c r="G51" s="3">
         <v>799</v>
       </c>
-      <c r="H51" s="4">
+      <c r="H51" s="3">
         <v>392</v>
       </c>
     </row>
@@ -8028,22 +8035,22 @@
       <c r="A52" s="1">
         <v>51</v>
       </c>
-      <c r="B52" s="2">
+      <c r="B52">
         <v>836</v>
       </c>
-      <c r="C52" s="2">
+      <c r="C52">
         <v>815</v>
       </c>
       <c r="D52">
         <v>400</v>
       </c>
-      <c r="F52" s="4">
+      <c r="F52" s="3">
         <v>836</v>
       </c>
-      <c r="G52" s="4">
+      <c r="G52" s="3">
         <v>815</v>
       </c>
-      <c r="H52" s="4">
+      <c r="H52" s="3">
         <v>400</v>
       </c>
     </row>
@@ -8051,22 +8058,22 @@
       <c r="A53" s="1">
         <v>52</v>
       </c>
-      <c r="B53" s="2">
+      <c r="B53">
         <v>816</v>
       </c>
-      <c r="C53" s="2">
+      <c r="C53">
         <v>831</v>
       </c>
       <c r="D53">
         <v>408</v>
       </c>
-      <c r="F53" s="4">
+      <c r="F53" s="3">
         <v>816</v>
       </c>
-      <c r="G53" s="4">
+      <c r="G53" s="3">
         <v>831</v>
       </c>
-      <c r="H53" s="4">
+      <c r="H53" s="3">
         <v>408</v>
       </c>
     </row>
@@ -8074,22 +8081,22 @@
       <c r="A54" s="1">
         <v>53</v>
       </c>
-      <c r="B54" s="2">
+      <c r="B54">
         <v>796</v>
       </c>
-      <c r="C54" s="2">
+      <c r="C54">
         <v>847</v>
       </c>
       <c r="D54">
         <v>416</v>
       </c>
-      <c r="F54" s="4">
+      <c r="F54" s="3">
         <v>796</v>
       </c>
-      <c r="G54" s="4">
+      <c r="G54" s="3">
         <v>847</v>
       </c>
-      <c r="H54" s="4">
+      <c r="H54" s="3">
         <v>416</v>
       </c>
     </row>
@@ -8097,22 +8104,22 @@
       <c r="A55" s="1">
         <v>54</v>
       </c>
-      <c r="B55" s="2">
+      <c r="B55">
         <v>774</v>
       </c>
-      <c r="C55" s="2">
+      <c r="C55">
         <v>863</v>
       </c>
       <c r="D55">
         <v>424</v>
       </c>
-      <c r="F55" s="4">
+      <c r="F55" s="3">
         <v>774</v>
       </c>
-      <c r="G55" s="4">
+      <c r="G55" s="3">
         <v>863</v>
       </c>
-      <c r="H55" s="4">
+      <c r="H55" s="3">
         <v>424</v>
       </c>
     </row>
@@ -8120,22 +8127,22 @@
       <c r="A56" s="1">
         <v>55</v>
       </c>
-      <c r="B56" s="2">
+      <c r="B56">
         <v>753</v>
       </c>
-      <c r="C56" s="2">
+      <c r="C56">
         <v>879</v>
       </c>
       <c r="D56">
         <v>432</v>
       </c>
-      <c r="F56" s="4">
+      <c r="F56" s="3">
         <v>753</v>
       </c>
-      <c r="G56" s="4">
+      <c r="G56" s="3">
         <v>879</v>
       </c>
-      <c r="H56" s="4">
+      <c r="H56" s="3">
         <v>432</v>
       </c>
     </row>
@@ -8143,22 +8150,22 @@
       <c r="A57" s="1">
         <v>56</v>
       </c>
-      <c r="B57" s="2">
+      <c r="B57">
         <v>730</v>
       </c>
-      <c r="C57" s="2">
+      <c r="C57">
         <v>895</v>
       </c>
       <c r="D57">
         <v>440</v>
       </c>
-      <c r="F57" s="4">
+      <c r="F57" s="3">
         <v>730</v>
       </c>
-      <c r="G57" s="4">
+      <c r="G57" s="3">
         <v>895</v>
       </c>
-      <c r="H57" s="4">
+      <c r="H57" s="3">
         <v>440</v>
       </c>
     </row>
@@ -8166,22 +8173,22 @@
       <c r="A58" s="1">
         <v>57</v>
       </c>
-      <c r="B58" s="2">
+      <c r="B58">
         <v>707</v>
       </c>
-      <c r="C58" s="2">
+      <c r="C58">
         <v>911</v>
       </c>
       <c r="D58">
         <v>448</v>
       </c>
-      <c r="F58" s="4">
+      <c r="F58" s="3">
         <v>707</v>
       </c>
-      <c r="G58" s="4">
+      <c r="G58" s="3">
         <v>911</v>
       </c>
-      <c r="H58" s="4">
+      <c r="H58" s="3">
         <v>448</v>
       </c>
     </row>
@@ -8189,22 +8196,22 @@
       <c r="A59" s="1">
         <v>58</v>
       </c>
-      <c r="B59" s="2">
+      <c r="B59">
         <v>684</v>
       </c>
-      <c r="C59" s="2">
+      <c r="C59">
         <v>927</v>
       </c>
       <c r="D59">
         <v>456</v>
       </c>
-      <c r="F59" s="4">
+      <c r="F59" s="3">
         <v>684</v>
       </c>
-      <c r="G59" s="4">
+      <c r="G59" s="3">
         <v>927</v>
       </c>
-      <c r="H59" s="4">
+      <c r="H59" s="3">
         <v>456</v>
       </c>
     </row>
@@ -8212,22 +8219,22 @@
       <c r="A60" s="1">
         <v>59</v>
       </c>
-      <c r="B60" s="2">
+      <c r="B60">
         <v>660</v>
       </c>
-      <c r="C60" s="2">
+      <c r="C60">
         <v>943</v>
       </c>
       <c r="D60">
         <v>464</v>
       </c>
-      <c r="F60" s="4">
+      <c r="F60" s="3">
         <v>660</v>
       </c>
-      <c r="G60" s="4">
+      <c r="G60" s="3">
         <v>943</v>
       </c>
-      <c r="H60" s="4">
+      <c r="H60" s="3">
         <v>464</v>
       </c>
     </row>
@@ -8235,22 +8242,22 @@
       <c r="A61" s="1">
         <v>60</v>
       </c>
-      <c r="B61" s="2">
+      <c r="B61">
         <v>636</v>
       </c>
-      <c r="C61" s="2">
+      <c r="C61">
         <v>959</v>
       </c>
       <c r="D61">
         <v>472</v>
       </c>
-      <c r="F61" s="4">
+      <c r="F61" s="3">
         <v>636</v>
       </c>
-      <c r="G61" s="4">
+      <c r="G61" s="3">
         <v>959</v>
       </c>
-      <c r="H61" s="4">
+      <c r="H61" s="3">
         <v>472</v>
       </c>
     </row>
@@ -8258,22 +8265,22 @@
       <c r="A62" s="1">
         <v>61</v>
       </c>
-      <c r="B62" s="2">
+      <c r="B62">
         <v>611</v>
       </c>
-      <c r="C62" s="2">
+      <c r="C62">
         <v>975</v>
       </c>
       <c r="D62">
         <v>480</v>
       </c>
-      <c r="F62" s="4">
+      <c r="F62" s="3">
         <v>611</v>
       </c>
-      <c r="G62" s="4">
+      <c r="G62" s="3">
         <v>975</v>
       </c>
-      <c r="H62" s="4">
+      <c r="H62" s="3">
         <v>480</v>
       </c>
     </row>
@@ -8281,22 +8288,22 @@
       <c r="A63" s="1">
         <v>62</v>
       </c>
-      <c r="B63" s="2">
+      <c r="B63">
         <v>587</v>
       </c>
-      <c r="C63" s="2">
+      <c r="C63">
         <v>991</v>
       </c>
       <c r="D63">
         <v>488</v>
       </c>
-      <c r="F63" s="4">
+      <c r="F63" s="3">
         <v>587</v>
       </c>
-      <c r="G63" s="4">
+      <c r="G63" s="3">
         <v>991</v>
       </c>
-      <c r="H63" s="4">
+      <c r="H63" s="3">
         <v>488</v>
       </c>
     </row>
@@ -8304,22 +8311,22 @@
       <c r="A64" s="1">
         <v>63</v>
       </c>
-      <c r="B64" s="2">
+      <c r="B64">
         <v>562</v>
       </c>
-      <c r="C64" s="2">
+      <c r="C64">
         <v>1007</v>
       </c>
       <c r="D64">
         <v>496</v>
       </c>
-      <c r="F64" s="4">
+      <c r="F64" s="3">
         <v>562</v>
       </c>
-      <c r="G64" s="4">
+      <c r="G64" s="3">
         <v>1007</v>
       </c>
-      <c r="H64" s="4">
+      <c r="H64" s="3">
         <v>496</v>
       </c>
     </row>
@@ -8327,22 +8334,22 @@
       <c r="A65" s="1">
         <v>64</v>
       </c>
-      <c r="B65" s="2">
+      <c r="B65">
         <v>537</v>
       </c>
-      <c r="C65" s="2">
+      <c r="C65">
         <v>1023</v>
       </c>
       <c r="D65">
         <v>504</v>
       </c>
-      <c r="F65" s="4">
+      <c r="F65" s="3">
         <v>537</v>
       </c>
-      <c r="G65" s="4">
+      <c r="G65" s="3">
         <v>1023</v>
       </c>
-      <c r="H65" s="4">
+      <c r="H65" s="3">
         <v>504</v>
       </c>
     </row>
@@ -8350,22 +8357,22 @@
       <c r="A66" s="1">
         <v>65</v>
       </c>
-      <c r="B66" s="2">
+      <c r="B66">
         <v>512</v>
       </c>
-      <c r="C66" s="2">
+      <c r="C66">
         <v>1007</v>
       </c>
       <c r="D66">
         <v>512</v>
       </c>
-      <c r="F66" s="4">
+      <c r="F66" s="3">
         <v>512</v>
       </c>
-      <c r="G66" s="4">
+      <c r="G66" s="3">
         <v>1007</v>
       </c>
-      <c r="H66" s="4">
+      <c r="H66" s="3">
         <v>512</v>
       </c>
     </row>
@@ -8373,22 +8380,22 @@
       <c r="A67" s="1">
         <v>66</v>
       </c>
-      <c r="B67" s="2">
+      <c r="B67">
         <v>486</v>
       </c>
-      <c r="C67" s="2">
+      <c r="C67">
         <v>991</v>
       </c>
       <c r="D67">
         <v>520</v>
       </c>
-      <c r="F67" s="4">
+      <c r="F67" s="3">
         <v>486</v>
       </c>
-      <c r="G67" s="4">
+      <c r="G67" s="3">
         <v>991</v>
       </c>
-      <c r="H67" s="4">
+      <c r="H67" s="3">
         <v>520</v>
       </c>
     </row>
@@ -8396,22 +8403,22 @@
       <c r="A68" s="1">
         <v>67</v>
       </c>
-      <c r="B68" s="2">
+      <c r="B68">
         <v>461</v>
       </c>
-      <c r="C68" s="2">
+      <c r="C68">
         <v>975</v>
       </c>
       <c r="D68">
         <v>528</v>
       </c>
-      <c r="F68" s="4">
+      <c r="F68" s="3">
         <v>461</v>
       </c>
-      <c r="G68" s="4">
+      <c r="G68" s="3">
         <v>975</v>
       </c>
-      <c r="H68" s="4">
+      <c r="H68" s="3">
         <v>528</v>
       </c>
     </row>
@@ -8419,22 +8426,22 @@
       <c r="A69" s="1">
         <v>68</v>
       </c>
-      <c r="B69" s="2">
+      <c r="B69">
         <v>436</v>
       </c>
-      <c r="C69" s="2">
+      <c r="C69">
         <v>959</v>
       </c>
       <c r="D69">
         <v>536</v>
       </c>
-      <c r="F69" s="4">
+      <c r="F69" s="3">
         <v>436</v>
       </c>
-      <c r="G69" s="4">
+      <c r="G69" s="3">
         <v>959</v>
       </c>
-      <c r="H69" s="4">
+      <c r="H69" s="3">
         <v>536</v>
       </c>
     </row>
@@ -8442,22 +8449,22 @@
       <c r="A70" s="1">
         <v>69</v>
       </c>
-      <c r="B70" s="2">
+      <c r="B70">
         <v>412</v>
       </c>
-      <c r="C70" s="2">
+      <c r="C70">
         <v>943</v>
       </c>
       <c r="D70">
         <v>544</v>
       </c>
-      <c r="F70" s="4">
+      <c r="F70" s="3">
         <v>412</v>
       </c>
-      <c r="G70" s="4">
+      <c r="G70" s="3">
         <v>943</v>
       </c>
-      <c r="H70" s="4">
+      <c r="H70" s="3">
         <v>544</v>
       </c>
     </row>
@@ -8465,22 +8472,22 @@
       <c r="A71" s="1">
         <v>70</v>
       </c>
-      <c r="B71" s="2">
+      <c r="B71">
         <v>387</v>
       </c>
-      <c r="C71" s="2">
+      <c r="C71">
         <v>927</v>
       </c>
       <c r="D71">
         <v>552</v>
       </c>
-      <c r="F71" s="4">
+      <c r="F71" s="3">
         <v>387</v>
       </c>
-      <c r="G71" s="4">
+      <c r="G71" s="3">
         <v>927</v>
       </c>
-      <c r="H71" s="4">
+      <c r="H71" s="3">
         <v>552</v>
       </c>
     </row>
@@ -8488,22 +8495,22 @@
       <c r="A72" s="1">
         <v>71</v>
       </c>
-      <c r="B72" s="2">
+      <c r="B72">
         <v>363</v>
       </c>
-      <c r="C72" s="2">
+      <c r="C72">
         <v>911</v>
       </c>
       <c r="D72">
         <v>560</v>
       </c>
-      <c r="F72" s="4">
+      <c r="F72" s="3">
         <v>363</v>
       </c>
-      <c r="G72" s="4">
+      <c r="G72" s="3">
         <v>911</v>
       </c>
-      <c r="H72" s="4">
+      <c r="H72" s="3">
         <v>560</v>
       </c>
     </row>
@@ -8511,22 +8518,22 @@
       <c r="A73" s="1">
         <v>72</v>
       </c>
-      <c r="B73" s="2">
+      <c r="B73">
         <v>339</v>
       </c>
-      <c r="C73" s="2">
+      <c r="C73">
         <v>895</v>
       </c>
       <c r="D73">
         <v>568</v>
       </c>
-      <c r="F73" s="4">
+      <c r="F73" s="3">
         <v>339</v>
       </c>
-      <c r="G73" s="4">
+      <c r="G73" s="3">
         <v>895</v>
       </c>
-      <c r="H73" s="4">
+      <c r="H73" s="3">
         <v>568</v>
       </c>
     </row>
@@ -8534,22 +8541,22 @@
       <c r="A74" s="1">
         <v>73</v>
       </c>
-      <c r="B74" s="2">
+      <c r="B74">
         <v>316</v>
       </c>
-      <c r="C74" s="2">
+      <c r="C74">
         <v>879</v>
       </c>
       <c r="D74">
         <v>576</v>
       </c>
-      <c r="F74" s="4">
+      <c r="F74" s="3">
         <v>316</v>
       </c>
-      <c r="G74" s="4">
+      <c r="G74" s="3">
         <v>879</v>
       </c>
-      <c r="H74" s="4">
+      <c r="H74" s="3">
         <v>576</v>
       </c>
     </row>
@@ -8557,22 +8564,22 @@
       <c r="A75" s="1">
         <v>74</v>
       </c>
-      <c r="B75" s="2">
+      <c r="B75">
         <v>293</v>
       </c>
-      <c r="C75" s="2">
+      <c r="C75">
         <v>863</v>
       </c>
       <c r="D75">
         <v>584</v>
       </c>
-      <c r="F75" s="4">
+      <c r="F75" s="3">
         <v>293</v>
       </c>
-      <c r="G75" s="4">
+      <c r="G75" s="3">
         <v>863</v>
       </c>
-      <c r="H75" s="4">
+      <c r="H75" s="3">
         <v>584</v>
       </c>
     </row>
@@ -8580,22 +8587,22 @@
       <c r="A76" s="1">
         <v>75</v>
       </c>
-      <c r="B76" s="2">
+      <c r="B76">
         <v>270</v>
       </c>
-      <c r="C76" s="2">
+      <c r="C76">
         <v>847</v>
       </c>
       <c r="D76">
         <v>592</v>
       </c>
-      <c r="F76" s="4">
+      <c r="F76" s="3">
         <v>270</v>
       </c>
-      <c r="G76" s="4">
+      <c r="G76" s="3">
         <v>847</v>
       </c>
-      <c r="H76" s="4">
+      <c r="H76" s="3">
         <v>592</v>
       </c>
     </row>
@@ -8603,22 +8610,22 @@
       <c r="A77" s="1">
         <v>76</v>
       </c>
-      <c r="B77" s="2">
+      <c r="B77">
         <v>249</v>
       </c>
-      <c r="C77" s="2">
+      <c r="C77">
         <v>831</v>
       </c>
       <c r="D77">
         <v>600</v>
       </c>
-      <c r="F77" s="4">
+      <c r="F77" s="3">
         <v>249</v>
       </c>
-      <c r="G77" s="4">
+      <c r="G77" s="3">
         <v>831</v>
       </c>
-      <c r="H77" s="4">
+      <c r="H77" s="3">
         <v>600</v>
       </c>
     </row>
@@ -8626,22 +8633,22 @@
       <c r="A78" s="1">
         <v>77</v>
       </c>
-      <c r="B78" s="2">
+      <c r="B78">
         <v>227</v>
       </c>
-      <c r="C78" s="2">
+      <c r="C78">
         <v>815</v>
       </c>
       <c r="D78">
         <v>608</v>
       </c>
-      <c r="F78" s="4">
+      <c r="F78" s="3">
         <v>227</v>
       </c>
-      <c r="G78" s="4">
+      <c r="G78" s="3">
         <v>815</v>
       </c>
-      <c r="H78" s="4">
+      <c r="H78" s="3">
         <v>608</v>
       </c>
     </row>
@@ -8649,22 +8656,22 @@
       <c r="A79" s="1">
         <v>78</v>
       </c>
-      <c r="B79" s="2">
+      <c r="B79">
         <v>207</v>
       </c>
-      <c r="C79" s="2">
+      <c r="C79">
         <v>799</v>
       </c>
       <c r="D79">
         <v>616</v>
       </c>
-      <c r="F79" s="4">
+      <c r="F79" s="3">
         <v>207</v>
       </c>
-      <c r="G79" s="4">
+      <c r="G79" s="3">
         <v>799</v>
       </c>
-      <c r="H79" s="4">
+      <c r="H79" s="3">
         <v>616</v>
       </c>
     </row>
@@ -8672,22 +8679,22 @@
       <c r="A80" s="1">
         <v>79</v>
       </c>
-      <c r="B80" s="2">
+      <c r="B80">
         <v>187</v>
       </c>
-      <c r="C80" s="2">
+      <c r="C80">
         <v>783</v>
       </c>
       <c r="D80">
         <v>624</v>
       </c>
-      <c r="F80" s="4">
+      <c r="F80" s="3">
         <v>187</v>
       </c>
-      <c r="G80" s="4">
+      <c r="G80" s="3">
         <v>783</v>
       </c>
-      <c r="H80" s="4">
+      <c r="H80" s="3">
         <v>624</v>
       </c>
     </row>
@@ -8695,22 +8702,22 @@
       <c r="A81" s="1">
         <v>80</v>
       </c>
-      <c r="B81" s="2">
+      <c r="B81">
         <v>168</v>
       </c>
-      <c r="C81" s="2">
+      <c r="C81">
         <v>767</v>
       </c>
       <c r="D81">
         <v>632</v>
       </c>
-      <c r="F81" s="4">
+      <c r="F81" s="3">
         <v>168</v>
       </c>
-      <c r="G81" s="4">
+      <c r="G81" s="3">
         <v>767</v>
       </c>
-      <c r="H81" s="4">
+      <c r="H81" s="3">
         <v>632</v>
       </c>
     </row>
@@ -8718,22 +8725,22 @@
       <c r="A82" s="1">
         <v>81</v>
       </c>
-      <c r="B82" s="2">
+      <c r="B82">
         <v>150</v>
       </c>
-      <c r="C82" s="2">
+      <c r="C82">
         <v>751</v>
       </c>
       <c r="D82">
         <v>640</v>
       </c>
-      <c r="F82" s="4">
+      <c r="F82" s="3">
         <v>150</v>
       </c>
-      <c r="G82" s="4">
+      <c r="G82" s="3">
         <v>751</v>
       </c>
-      <c r="H82" s="4">
+      <c r="H82" s="3">
         <v>640</v>
       </c>
     </row>
@@ -8741,22 +8748,22 @@
       <c r="A83" s="1">
         <v>82</v>
       </c>
-      <c r="B83" s="2">
+      <c r="B83">
         <v>133</v>
       </c>
-      <c r="C83" s="2">
+      <c r="C83">
         <v>735</v>
       </c>
       <c r="D83">
         <v>648</v>
       </c>
-      <c r="F83" s="4">
+      <c r="F83" s="3">
         <v>133</v>
       </c>
-      <c r="G83" s="4">
+      <c r="G83" s="3">
         <v>735</v>
       </c>
-      <c r="H83" s="4">
+      <c r="H83" s="3">
         <v>648</v>
       </c>
     </row>
@@ -8764,22 +8771,22 @@
       <c r="A84" s="1">
         <v>83</v>
       </c>
-      <c r="B84" s="2">
+      <c r="B84">
         <v>116</v>
       </c>
-      <c r="C84" s="2">
+      <c r="C84">
         <v>719</v>
       </c>
       <c r="D84">
         <v>656</v>
       </c>
-      <c r="F84" s="4">
+      <c r="F84" s="3">
         <v>116</v>
       </c>
-      <c r="G84" s="4">
+      <c r="G84" s="3">
         <v>719</v>
       </c>
-      <c r="H84" s="4">
+      <c r="H84" s="3">
         <v>656</v>
       </c>
     </row>
@@ -8787,22 +8794,22 @@
       <c r="A85" s="1">
         <v>84</v>
       </c>
-      <c r="B85" s="2">
+      <c r="B85">
         <v>101</v>
       </c>
-      <c r="C85" s="2">
+      <c r="C85">
         <v>703</v>
       </c>
       <c r="D85">
         <v>664</v>
       </c>
-      <c r="F85" s="4">
+      <c r="F85" s="3">
         <v>101</v>
       </c>
-      <c r="G85" s="4">
+      <c r="G85" s="3">
         <v>703</v>
       </c>
-      <c r="H85" s="4">
+      <c r="H85" s="3">
         <v>664</v>
       </c>
     </row>
@@ -8810,22 +8817,22 @@
       <c r="A86" s="1">
         <v>85</v>
       </c>
-      <c r="B86" s="2">
+      <c r="B86">
         <v>86</v>
       </c>
-      <c r="C86" s="2">
+      <c r="C86">
         <v>687</v>
       </c>
       <c r="D86">
         <v>672</v>
       </c>
-      <c r="F86" s="4">
+      <c r="F86" s="3">
         <v>86</v>
       </c>
-      <c r="G86" s="4">
+      <c r="G86" s="3">
         <v>687</v>
       </c>
-      <c r="H86" s="4">
+      <c r="H86" s="3">
         <v>672</v>
       </c>
     </row>
@@ -8833,22 +8840,22 @@
       <c r="A87" s="1">
         <v>86</v>
       </c>
-      <c r="B87" s="2">
+      <c r="B87">
         <v>73</v>
       </c>
-      <c r="C87" s="2">
+      <c r="C87">
         <v>671</v>
       </c>
       <c r="D87">
         <v>680</v>
       </c>
-      <c r="F87" s="4">
+      <c r="F87" s="3">
         <v>73</v>
       </c>
-      <c r="G87" s="4">
+      <c r="G87" s="3">
         <v>671</v>
       </c>
-      <c r="H87" s="4">
+      <c r="H87" s="3">
         <v>680</v>
       </c>
     </row>
@@ -8856,22 +8863,22 @@
       <c r="A88" s="1">
         <v>87</v>
       </c>
-      <c r="B88" s="2">
+      <c r="B88">
         <v>60</v>
       </c>
-      <c r="C88" s="2">
+      <c r="C88">
         <v>655</v>
       </c>
       <c r="D88">
         <v>688</v>
       </c>
-      <c r="F88" s="4">
+      <c r="F88" s="3">
         <v>60</v>
       </c>
-      <c r="G88" s="4">
+      <c r="G88" s="3">
         <v>655</v>
       </c>
-      <c r="H88" s="4">
+      <c r="H88" s="3">
         <v>688</v>
       </c>
     </row>
@@ -8879,22 +8886,22 @@
       <c r="A89" s="1">
         <v>88</v>
       </c>
-      <c r="B89" s="2">
+      <c r="B89">
         <v>49</v>
       </c>
-      <c r="C89" s="2">
+      <c r="C89">
         <v>639</v>
       </c>
       <c r="D89">
         <v>696</v>
       </c>
-      <c r="F89" s="4">
+      <c r="F89" s="3">
         <v>49</v>
       </c>
-      <c r="G89" s="4">
+      <c r="G89" s="3">
         <v>639</v>
       </c>
-      <c r="H89" s="4">
+      <c r="H89" s="3">
         <v>696</v>
       </c>
     </row>
@@ -8902,22 +8909,22 @@
       <c r="A90" s="1">
         <v>89</v>
       </c>
-      <c r="B90" s="2">
+      <c r="B90">
         <v>39</v>
       </c>
-      <c r="C90" s="2">
+      <c r="C90">
         <v>623</v>
       </c>
       <c r="D90">
         <v>704</v>
       </c>
-      <c r="F90" s="4">
+      <c r="F90" s="3">
         <v>39</v>
       </c>
-      <c r="G90" s="4">
+      <c r="G90" s="3">
         <v>623</v>
       </c>
-      <c r="H90" s="4">
+      <c r="H90" s="3">
         <v>704</v>
       </c>
     </row>
@@ -8925,22 +8932,22 @@
       <c r="A91" s="1">
         <v>90</v>
       </c>
-      <c r="B91" s="2">
+      <c r="B91">
         <v>30</v>
       </c>
-      <c r="C91" s="2">
+      <c r="C91">
         <v>607</v>
       </c>
       <c r="D91">
         <v>712</v>
       </c>
-      <c r="F91" s="4">
+      <c r="F91" s="3">
         <v>30</v>
       </c>
-      <c r="G91" s="4">
+      <c r="G91" s="3">
         <v>607</v>
       </c>
-      <c r="H91" s="4">
+      <c r="H91" s="3">
         <v>712</v>
       </c>
     </row>
@@ -8948,22 +8955,22 @@
       <c r="A92" s="1">
         <v>91</v>
       </c>
-      <c r="B92" s="2">
+      <c r="B92">
         <v>22</v>
       </c>
-      <c r="C92" s="2">
+      <c r="C92">
         <v>591</v>
       </c>
       <c r="D92">
         <v>720</v>
       </c>
-      <c r="F92" s="4">
+      <c r="F92" s="3">
         <v>22</v>
       </c>
-      <c r="G92" s="4">
+      <c r="G92" s="3">
         <v>591</v>
       </c>
-      <c r="H92" s="4">
+      <c r="H92" s="3">
         <v>720</v>
       </c>
     </row>
@@ -8971,22 +8978,22 @@
       <c r="A93" s="1">
         <v>92</v>
       </c>
-      <c r="B93" s="2">
+      <c r="B93">
         <v>15</v>
       </c>
-      <c r="C93" s="2">
+      <c r="C93">
         <v>575</v>
       </c>
       <c r="D93">
         <v>728</v>
       </c>
-      <c r="F93" s="4">
+      <c r="F93" s="3">
         <v>15</v>
       </c>
-      <c r="G93" s="4">
+      <c r="G93" s="3">
         <v>575</v>
       </c>
-      <c r="H93" s="4">
+      <c r="H93" s="3">
         <v>728</v>
       </c>
     </row>
@@ -8994,22 +9001,22 @@
       <c r="A94" s="1">
         <v>93</v>
       </c>
-      <c r="B94" s="2">
+      <c r="B94">
         <v>10</v>
       </c>
-      <c r="C94" s="2">
+      <c r="C94">
         <v>559</v>
       </c>
       <c r="D94">
         <v>736</v>
       </c>
-      <c r="F94" s="4">
+      <c r="F94" s="3">
         <v>10</v>
       </c>
-      <c r="G94" s="4">
+      <c r="G94" s="3">
         <v>559</v>
       </c>
-      <c r="H94" s="4">
+      <c r="H94" s="3">
         <v>736</v>
       </c>
     </row>
@@ -9017,22 +9024,22 @@
       <c r="A95" s="1">
         <v>94</v>
       </c>
-      <c r="B95" s="2">
+      <c r="B95">
         <v>6</v>
       </c>
-      <c r="C95" s="2">
+      <c r="C95">
         <v>543</v>
       </c>
       <c r="D95">
         <v>744</v>
       </c>
-      <c r="F95" s="4">
+      <c r="F95" s="3">
         <v>6</v>
       </c>
-      <c r="G95" s="4">
+      <c r="G95" s="3">
         <v>543</v>
       </c>
-      <c r="H95" s="4">
+      <c r="H95" s="3">
         <v>744</v>
       </c>
     </row>
@@ -9040,22 +9047,22 @@
       <c r="A96" s="1">
         <v>95</v>
       </c>
-      <c r="B96" s="2">
+      <c r="B96">
         <v>2</v>
       </c>
-      <c r="C96" s="2">
+      <c r="C96">
         <v>527</v>
       </c>
       <c r="D96">
         <v>752</v>
       </c>
-      <c r="F96" s="4">
+      <c r="F96" s="3">
         <v>2</v>
       </c>
-      <c r="G96" s="4">
+      <c r="G96" s="3">
         <v>527</v>
       </c>
-      <c r="H96" s="4">
+      <c r="H96" s="3">
         <v>752</v>
       </c>
     </row>
@@ -9063,22 +9070,22 @@
       <c r="A97" s="1">
         <v>96</v>
       </c>
-      <c r="B97" s="2">
+      <c r="B97">
         <v>1</v>
       </c>
-      <c r="C97" s="2">
+      <c r="C97">
         <v>512</v>
       </c>
       <c r="D97">
         <v>760</v>
       </c>
-      <c r="F97" s="4">
+      <c r="F97" s="3">
         <v>1</v>
       </c>
-      <c r="G97" s="4">
+      <c r="G97" s="3">
         <v>512</v>
       </c>
-      <c r="H97" s="4">
+      <c r="H97" s="3">
         <v>760</v>
       </c>
     </row>
@@ -9086,22 +9093,22 @@
       <c r="A98" s="1">
         <v>97</v>
       </c>
-      <c r="B98" s="2">
+      <c r="B98">
         <v>0</v>
       </c>
-      <c r="C98" s="2">
+      <c r="C98">
         <v>496</v>
       </c>
       <c r="D98">
         <v>768</v>
       </c>
-      <c r="F98" s="4">
+      <c r="F98" s="3">
         <v>0</v>
       </c>
-      <c r="G98" s="4">
+      <c r="G98" s="3">
         <v>496</v>
       </c>
-      <c r="H98" s="4">
+      <c r="H98" s="3">
         <v>768</v>
       </c>
     </row>
@@ -9109,22 +9116,22 @@
       <c r="A99" s="1">
         <v>98</v>
       </c>
-      <c r="B99" s="2">
+      <c r="B99">
         <v>1</v>
       </c>
-      <c r="C99" s="2">
+      <c r="C99">
         <v>480</v>
       </c>
       <c r="D99">
         <v>776</v>
       </c>
-      <c r="F99" s="4">
+      <c r="F99" s="3">
         <v>1</v>
       </c>
-      <c r="G99" s="4">
+      <c r="G99" s="3">
         <v>480</v>
       </c>
-      <c r="H99" s="4">
+      <c r="H99" s="3">
         <v>776</v>
       </c>
     </row>
@@ -9132,22 +9139,22 @@
       <c r="A100" s="1">
         <v>99</v>
       </c>
-      <c r="B100" s="2">
+      <c r="B100">
         <v>2</v>
       </c>
-      <c r="C100" s="2">
+      <c r="C100">
         <v>464</v>
       </c>
       <c r="D100">
         <v>784</v>
       </c>
-      <c r="F100" s="4">
+      <c r="F100" s="3">
         <v>2</v>
       </c>
-      <c r="G100" s="4">
+      <c r="G100" s="3">
         <v>464</v>
       </c>
-      <c r="H100" s="4">
+      <c r="H100" s="3">
         <v>784</v>
       </c>
     </row>
@@ -9155,22 +9162,22 @@
       <c r="A101" s="1">
         <v>100</v>
       </c>
-      <c r="B101" s="2">
+      <c r="B101">
         <v>6</v>
       </c>
-      <c r="C101" s="2">
+      <c r="C101">
         <v>448</v>
       </c>
       <c r="D101">
         <v>792</v>
       </c>
-      <c r="F101" s="4">
+      <c r="F101" s="3">
         <v>6</v>
       </c>
-      <c r="G101" s="4">
+      <c r="G101" s="3">
         <v>448</v>
       </c>
-      <c r="H101" s="4">
+      <c r="H101" s="3">
         <v>792</v>
       </c>
     </row>
@@ -9178,22 +9185,22 @@
       <c r="A102" s="1">
         <v>101</v>
       </c>
-      <c r="B102" s="2">
+      <c r="B102">
         <v>10</v>
       </c>
-      <c r="C102" s="2">
+      <c r="C102">
         <v>432</v>
       </c>
       <c r="D102">
         <v>800</v>
       </c>
-      <c r="F102" s="4">
+      <c r="F102" s="3">
         <v>10</v>
       </c>
-      <c r="G102" s="4">
+      <c r="G102" s="3">
         <v>432</v>
       </c>
-      <c r="H102" s="4">
+      <c r="H102" s="3">
         <v>800</v>
       </c>
     </row>
@@ -9201,22 +9208,22 @@
       <c r="A103" s="1">
         <v>102</v>
       </c>
-      <c r="B103" s="2">
+      <c r="B103">
         <v>15</v>
       </c>
-      <c r="C103" s="2">
+      <c r="C103">
         <v>416</v>
       </c>
       <c r="D103">
         <v>808</v>
       </c>
-      <c r="F103" s="4">
+      <c r="F103" s="3">
         <v>15</v>
       </c>
-      <c r="G103" s="4">
+      <c r="G103" s="3">
         <v>416</v>
       </c>
-      <c r="H103" s="4">
+      <c r="H103" s="3">
         <v>808</v>
       </c>
     </row>
@@ -9224,22 +9231,22 @@
       <c r="A104" s="1">
         <v>103</v>
       </c>
-      <c r="B104" s="2">
+      <c r="B104">
         <v>22</v>
       </c>
-      <c r="C104" s="2">
+      <c r="C104">
         <v>400</v>
       </c>
       <c r="D104">
         <v>816</v>
       </c>
-      <c r="F104" s="4">
+      <c r="F104" s="3">
         <v>22</v>
       </c>
-      <c r="G104" s="4">
+      <c r="G104" s="3">
         <v>400</v>
       </c>
-      <c r="H104" s="4">
+      <c r="H104" s="3">
         <v>816</v>
       </c>
     </row>
@@ -9247,22 +9254,22 @@
       <c r="A105" s="1">
         <v>104</v>
       </c>
-      <c r="B105" s="2">
+      <c r="B105">
         <v>30</v>
       </c>
-      <c r="C105" s="2">
+      <c r="C105">
         <v>384</v>
       </c>
       <c r="D105">
         <v>824</v>
       </c>
-      <c r="F105" s="4">
+      <c r="F105" s="3">
         <v>30</v>
       </c>
-      <c r="G105" s="4">
+      <c r="G105" s="3">
         <v>384</v>
       </c>
-      <c r="H105" s="4">
+      <c r="H105" s="3">
         <v>824</v>
       </c>
     </row>
@@ -9270,22 +9277,22 @@
       <c r="A106" s="1">
         <v>105</v>
       </c>
-      <c r="B106" s="2">
+      <c r="B106">
         <v>39</v>
       </c>
-      <c r="C106" s="2">
+      <c r="C106">
         <v>368</v>
       </c>
       <c r="D106">
         <v>832</v>
       </c>
-      <c r="F106" s="4">
+      <c r="F106" s="3">
         <v>39</v>
       </c>
-      <c r="G106" s="4">
+      <c r="G106" s="3">
         <v>368</v>
       </c>
-      <c r="H106" s="4">
+      <c r="H106" s="3">
         <v>832</v>
       </c>
     </row>
@@ -9293,22 +9300,22 @@
       <c r="A107" s="1">
         <v>106</v>
       </c>
-      <c r="B107" s="2">
+      <c r="B107">
         <v>49</v>
       </c>
-      <c r="C107" s="2">
+      <c r="C107">
         <v>352</v>
       </c>
       <c r="D107">
         <v>840</v>
       </c>
-      <c r="F107" s="4">
+      <c r="F107" s="3">
         <v>49</v>
       </c>
-      <c r="G107" s="4">
+      <c r="G107" s="3">
         <v>352</v>
       </c>
-      <c r="H107" s="4">
+      <c r="H107" s="3">
         <v>840</v>
       </c>
     </row>
@@ -9316,22 +9323,22 @@
       <c r="A108" s="1">
         <v>107</v>
       </c>
-      <c r="B108" s="2">
+      <c r="B108">
         <v>60</v>
       </c>
-      <c r="C108" s="2">
+      <c r="C108">
         <v>336</v>
       </c>
       <c r="D108">
         <v>848</v>
       </c>
-      <c r="F108" s="4">
+      <c r="F108" s="3">
         <v>60</v>
       </c>
-      <c r="G108" s="4">
+      <c r="G108" s="3">
         <v>336</v>
       </c>
-      <c r="H108" s="4">
+      <c r="H108" s="3">
         <v>848</v>
       </c>
     </row>
@@ -9339,22 +9346,22 @@
       <c r="A109" s="1">
         <v>108</v>
       </c>
-      <c r="B109" s="2">
+      <c r="B109">
         <v>73</v>
       </c>
-      <c r="C109" s="2">
+      <c r="C109">
         <v>320</v>
       </c>
       <c r="D109">
         <v>856</v>
       </c>
-      <c r="F109" s="4">
+      <c r="F109" s="3">
         <v>73</v>
       </c>
-      <c r="G109" s="4">
+      <c r="G109" s="3">
         <v>320</v>
       </c>
-      <c r="H109" s="4">
+      <c r="H109" s="3">
         <v>856</v>
       </c>
     </row>
@@ -9362,22 +9369,22 @@
       <c r="A110" s="1">
         <v>109</v>
       </c>
-      <c r="B110" s="2">
+      <c r="B110">
         <v>86</v>
       </c>
-      <c r="C110" s="2">
+      <c r="C110">
         <v>304</v>
       </c>
       <c r="D110">
         <v>864</v>
       </c>
-      <c r="F110" s="4">
+      <c r="F110" s="3">
         <v>86</v>
       </c>
-      <c r="G110" s="4">
+      <c r="G110" s="3">
         <v>304</v>
       </c>
-      <c r="H110" s="4">
+      <c r="H110" s="3">
         <v>864</v>
       </c>
     </row>
@@ -9385,22 +9392,22 @@
       <c r="A111" s="1">
         <v>110</v>
       </c>
-      <c r="B111" s="2">
+      <c r="B111">
         <v>101</v>
       </c>
-      <c r="C111" s="2">
+      <c r="C111">
         <v>288</v>
       </c>
       <c r="D111">
         <v>872</v>
       </c>
-      <c r="F111" s="4">
+      <c r="F111" s="3">
         <v>101</v>
       </c>
-      <c r="G111" s="4">
+      <c r="G111" s="3">
         <v>288</v>
       </c>
-      <c r="H111" s="4">
+      <c r="H111" s="3">
         <v>872</v>
       </c>
     </row>
@@ -9408,22 +9415,22 @@
       <c r="A112" s="1">
         <v>111</v>
       </c>
-      <c r="B112" s="2">
+      <c r="B112">
         <v>116</v>
       </c>
-      <c r="C112" s="2">
+      <c r="C112">
         <v>272</v>
       </c>
       <c r="D112">
         <v>880</v>
       </c>
-      <c r="F112" s="4">
+      <c r="F112" s="3">
         <v>116</v>
       </c>
-      <c r="G112" s="4">
+      <c r="G112" s="3">
         <v>272</v>
       </c>
-      <c r="H112" s="4">
+      <c r="H112" s="3">
         <v>880</v>
       </c>
     </row>
@@ -9431,22 +9438,22 @@
       <c r="A113" s="1">
         <v>112</v>
       </c>
-      <c r="B113" s="2">
+      <c r="B113">
         <v>133</v>
       </c>
-      <c r="C113" s="2">
+      <c r="C113">
         <v>256</v>
       </c>
       <c r="D113">
         <v>888</v>
       </c>
-      <c r="F113" s="4">
+      <c r="F113" s="3">
         <v>133</v>
       </c>
-      <c r="G113" s="4">
+      <c r="G113" s="3">
         <v>256</v>
       </c>
-      <c r="H113" s="4">
+      <c r="H113" s="3">
         <v>888</v>
       </c>
     </row>
@@ -9454,22 +9461,22 @@
       <c r="A114" s="1">
         <v>113</v>
       </c>
-      <c r="B114" s="2">
+      <c r="B114">
         <v>150</v>
       </c>
-      <c r="C114" s="2">
+      <c r="C114">
         <v>240</v>
       </c>
       <c r="D114">
         <v>896</v>
       </c>
-      <c r="F114" s="4">
+      <c r="F114" s="3">
         <v>150</v>
       </c>
-      <c r="G114" s="4">
+      <c r="G114" s="3">
         <v>240</v>
       </c>
-      <c r="H114" s="4">
+      <c r="H114" s="3">
         <v>896</v>
       </c>
     </row>
@@ -9477,22 +9484,22 @@
       <c r="A115" s="1">
         <v>114</v>
       </c>
-      <c r="B115" s="2">
+      <c r="B115">
         <v>168</v>
       </c>
-      <c r="C115" s="2">
+      <c r="C115">
         <v>224</v>
       </c>
       <c r="D115">
         <v>904</v>
       </c>
-      <c r="F115" s="4">
+      <c r="F115" s="3">
         <v>168</v>
       </c>
-      <c r="G115" s="4">
+      <c r="G115" s="3">
         <v>224</v>
       </c>
-      <c r="H115" s="4">
+      <c r="H115" s="3">
         <v>904</v>
       </c>
     </row>
@@ -9500,22 +9507,22 @@
       <c r="A116" s="1">
         <v>115</v>
       </c>
-      <c r="B116" s="2">
+      <c r="B116">
         <v>187</v>
       </c>
-      <c r="C116" s="2">
+      <c r="C116">
         <v>208</v>
       </c>
       <c r="D116">
         <v>912</v>
       </c>
-      <c r="F116" s="4">
+      <c r="F116" s="3">
         <v>187</v>
       </c>
-      <c r="G116" s="4">
+      <c r="G116" s="3">
         <v>208</v>
       </c>
-      <c r="H116" s="4">
+      <c r="H116" s="3">
         <v>912</v>
       </c>
     </row>
@@ -9523,22 +9530,22 @@
       <c r="A117" s="1">
         <v>116</v>
       </c>
-      <c r="B117" s="2">
+      <c r="B117">
         <v>207</v>
       </c>
-      <c r="C117" s="2">
+      <c r="C117">
         <v>192</v>
       </c>
       <c r="D117">
         <v>920</v>
       </c>
-      <c r="F117" s="4">
+      <c r="F117" s="3">
         <v>207</v>
       </c>
-      <c r="G117" s="4">
+      <c r="G117" s="3">
         <v>192</v>
       </c>
-      <c r="H117" s="4">
+      <c r="H117" s="3">
         <v>920</v>
       </c>
     </row>
@@ -9546,22 +9553,22 @@
       <c r="A118" s="1">
         <v>117</v>
       </c>
-      <c r="B118" s="2">
+      <c r="B118">
         <v>227</v>
       </c>
-      <c r="C118" s="2">
+      <c r="C118">
         <v>176</v>
       </c>
       <c r="D118">
         <v>928</v>
       </c>
-      <c r="F118" s="4">
+      <c r="F118" s="3">
         <v>227</v>
       </c>
-      <c r="G118" s="4">
+      <c r="G118" s="3">
         <v>176</v>
       </c>
-      <c r="H118" s="4">
+      <c r="H118" s="3">
         <v>928</v>
       </c>
     </row>
@@ -9569,22 +9576,22 @@
       <c r="A119" s="1">
         <v>118</v>
       </c>
-      <c r="B119" s="2">
+      <c r="B119">
         <v>249</v>
       </c>
-      <c r="C119" s="2">
+      <c r="C119">
         <v>160</v>
       </c>
       <c r="D119">
         <v>936</v>
       </c>
-      <c r="F119" s="4">
+      <c r="F119" s="3">
         <v>249</v>
       </c>
-      <c r="G119" s="4">
+      <c r="G119" s="3">
         <v>160</v>
       </c>
-      <c r="H119" s="4">
+      <c r="H119" s="3">
         <v>936</v>
       </c>
     </row>
@@ -9592,22 +9599,22 @@
       <c r="A120" s="1">
         <v>119</v>
       </c>
-      <c r="B120" s="2">
+      <c r="B120">
         <v>270</v>
       </c>
-      <c r="C120" s="2">
+      <c r="C120">
         <v>144</v>
       </c>
       <c r="D120">
         <v>944</v>
       </c>
-      <c r="F120" s="4">
+      <c r="F120" s="3">
         <v>270</v>
       </c>
-      <c r="G120" s="4">
+      <c r="G120" s="3">
         <v>144</v>
       </c>
-      <c r="H120" s="4">
+      <c r="H120" s="3">
         <v>944</v>
       </c>
     </row>
@@ -9615,22 +9622,22 @@
       <c r="A121" s="1">
         <v>120</v>
       </c>
-      <c r="B121" s="2">
+      <c r="B121">
         <v>293</v>
       </c>
-      <c r="C121" s="2">
+      <c r="C121">
         <v>128</v>
       </c>
       <c r="D121">
         <v>952</v>
       </c>
-      <c r="F121" s="4">
+      <c r="F121" s="3">
         <v>293</v>
       </c>
-      <c r="G121" s="4">
+      <c r="G121" s="3">
         <v>128</v>
       </c>
-      <c r="H121" s="4">
+      <c r="H121" s="3">
         <v>952</v>
       </c>
     </row>
@@ -9638,22 +9645,22 @@
       <c r="A122" s="1">
         <v>121</v>
       </c>
-      <c r="B122" s="2">
+      <c r="B122">
         <v>316</v>
       </c>
-      <c r="C122" s="2">
+      <c r="C122">
         <v>112</v>
       </c>
       <c r="D122">
         <v>960</v>
       </c>
-      <c r="F122" s="4">
+      <c r="F122" s="3">
         <v>316</v>
       </c>
-      <c r="G122" s="4">
+      <c r="G122" s="3">
         <v>112</v>
       </c>
-      <c r="H122" s="4">
+      <c r="H122" s="3">
         <v>960</v>
       </c>
     </row>
@@ -9661,22 +9668,22 @@
       <c r="A123" s="1">
         <v>122</v>
       </c>
-      <c r="B123" s="2">
+      <c r="B123">
         <v>339</v>
       </c>
-      <c r="C123" s="2">
+      <c r="C123">
         <v>96</v>
       </c>
       <c r="D123">
         <v>968</v>
       </c>
-      <c r="F123" s="4">
+      <c r="F123" s="3">
         <v>339</v>
       </c>
-      <c r="G123" s="4">
+      <c r="G123" s="3">
         <v>96</v>
       </c>
-      <c r="H123" s="4">
+      <c r="H123" s="3">
         <v>968</v>
       </c>
     </row>
@@ -9684,22 +9691,22 @@
       <c r="A124" s="1">
         <v>123</v>
       </c>
-      <c r="B124" s="2">
+      <c r="B124">
         <v>363</v>
       </c>
-      <c r="C124" s="2">
+      <c r="C124">
         <v>80</v>
       </c>
       <c r="D124">
         <v>976</v>
       </c>
-      <c r="F124" s="4">
+      <c r="F124" s="3">
         <v>363</v>
       </c>
-      <c r="G124" s="4">
+      <c r="G124" s="3">
         <v>80</v>
       </c>
-      <c r="H124" s="4">
+      <c r="H124" s="3">
         <v>976</v>
       </c>
     </row>
@@ -9707,22 +9714,22 @@
       <c r="A125" s="1">
         <v>124</v>
       </c>
-      <c r="B125" s="2">
+      <c r="B125">
         <v>387</v>
       </c>
-      <c r="C125" s="2">
+      <c r="C125">
         <v>64</v>
       </c>
       <c r="D125">
         <v>984</v>
       </c>
-      <c r="F125" s="4">
+      <c r="F125" s="3">
         <v>387</v>
       </c>
-      <c r="G125" s="4">
+      <c r="G125" s="3">
         <v>64</v>
       </c>
-      <c r="H125" s="4">
+      <c r="H125" s="3">
         <v>984</v>
       </c>
     </row>
@@ -9730,22 +9737,22 @@
       <c r="A126" s="1">
         <v>125</v>
       </c>
-      <c r="B126" s="2">
+      <c r="B126">
         <v>412</v>
       </c>
-      <c r="C126" s="2">
+      <c r="C126">
         <v>48</v>
       </c>
       <c r="D126">
         <v>992</v>
       </c>
-      <c r="F126" s="4">
+      <c r="F126" s="3">
         <v>412</v>
       </c>
-      <c r="G126" s="4">
+      <c r="G126" s="3">
         <v>48</v>
       </c>
-      <c r="H126" s="4">
+      <c r="H126" s="3">
         <v>992</v>
       </c>
     </row>
@@ -9753,22 +9760,22 @@
       <c r="A127" s="1">
         <v>126</v>
       </c>
-      <c r="B127" s="2">
+      <c r="B127">
         <v>436</v>
       </c>
-      <c r="C127" s="2">
+      <c r="C127">
         <v>32</v>
       </c>
       <c r="D127">
         <v>1000</v>
       </c>
-      <c r="F127" s="4">
+      <c r="F127" s="3">
         <v>436</v>
       </c>
-      <c r="G127" s="4">
+      <c r="G127" s="3">
         <v>32</v>
       </c>
-      <c r="H127" s="4">
+      <c r="H127" s="3">
         <v>1000</v>
       </c>
     </row>
@@ -9776,22 +9783,22 @@
       <c r="A128" s="1">
         <v>127</v>
       </c>
-      <c r="B128" s="2">
+      <c r="B128">
         <v>461</v>
       </c>
-      <c r="C128" s="2">
+      <c r="C128">
         <v>16</v>
       </c>
       <c r="D128">
         <v>1008</v>
       </c>
-      <c r="F128" s="4">
+      <c r="F128" s="3">
         <v>461</v>
       </c>
-      <c r="G128" s="4">
+      <c r="G128" s="3">
         <v>16</v>
       </c>
-      <c r="H128" s="4">
+      <c r="H128" s="3">
         <v>1008</v>
       </c>
     </row>
@@ -9799,22 +9806,22 @@
       <c r="A129" s="1">
         <v>128</v>
       </c>
-      <c r="B129" s="2">
+      <c r="B129">
         <v>486</v>
       </c>
-      <c r="C129" s="2">
+      <c r="C129">
         <v>0</v>
       </c>
       <c r="D129">
         <v>1016</v>
       </c>
-      <c r="F129" s="4">
+      <c r="F129" s="3">
         <v>486</v>
       </c>
-      <c r="G129" s="4">
+      <c r="G129" s="3">
         <v>0</v>
       </c>
-      <c r="H129" s="4">
+      <c r="H129" s="3">
         <v>1016</v>
       </c>
     </row>

</xml_diff>